<commit_message>
Update Test Case: Template (1), Template (2), Template (3)
</commit_message>
<xml_diff>
--- a/System 6 Renovation Working Files/Test Files/Template (2).xlsx
+++ b/System 6 Renovation Working Files/Test Files/Template (2).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
   <si>
     <t>BEGIN</t>
   </si>
@@ -273,6 +273,22 @@
   </si>
   <si>
     <t>Main Insured (Can be ignored if same as Policy Payer)</t>
+  </si>
+  <si>
+    <t>RATING_INDIVIDUAL-CBHIP4</t>
+  </si>
+  <si>
+    <t>RATING_INDIVIDUAL-CBHI02</t>
+  </si>
+  <si>
+    <t>RATING_INDIVIDUAL-CBHIP3</t>
+  </si>
+  <si>
+    <t>RATING_INDIVIDUAL-CBHI01</t>
+  </si>
+  <si>
+    <t>RATING_INDIVIDUAL-CBHIP4
+(Can ignore if holder is not insured)</t>
   </si>
 </sst>
 </file>
@@ -882,37 +898,37 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="62" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="61" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="62" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="62" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="61" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="46" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="62" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="33" borderId="10" xfId="62" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1278,7 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
       <selection activeCell="B93" sqref="B93:B101"/>
     </sheetView>
   </sheetViews>
@@ -1289,8 +1305,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3">
@@ -1301,8 +1317,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="3">
         <v>7</v>
       </c>
@@ -1311,8 +1327,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="6">
@@ -1323,8 +1339,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="24"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="5">
         <v>4</v>
       </c>
@@ -1333,8 +1349,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="5">
         <v>5</v>
       </c>
@@ -1343,8 +1359,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="5">
         <v>6</v>
       </c>
@@ -1353,8 +1369,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="5">
         <v>7</v>
       </c>
@@ -1363,7 +1379,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1375,8 +1391,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="6">
@@ -1387,8 +1403,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="5">
         <v>4</v>
       </c>
@@ -1397,8 +1413,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="5">
         <v>5</v>
       </c>
@@ -1407,8 +1423,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="5">
         <v>6</v>
       </c>
@@ -1417,8 +1433,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="24"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="5">
         <v>7</v>
       </c>
@@ -1427,8 +1443,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="24"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="6">
         <v>8</v>
       </c>
@@ -1437,8 +1453,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="25" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="8">
@@ -1449,8 +1465,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="8">
         <v>3</v>
       </c>
@@ -1459,8 +1475,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="26" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="30" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="10">
@@ -1471,8 +1487,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="10">
         <v>3</v>
       </c>
@@ -1481,8 +1497,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="26" t="s">
+      <c r="A19" s="24"/>
+      <c r="B19" s="30" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="10">
@@ -1493,8 +1509,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="10">
         <v>3</v>
       </c>
@@ -1503,10 +1519,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="13">
@@ -1517,8 +1533,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="27"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="13">
         <v>4</v>
       </c>
@@ -1527,8 +1543,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="12">
         <v>5</v>
       </c>
@@ -1537,8 +1553,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="27"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="12">
         <v>8</v>
       </c>
@@ -1547,8 +1563,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="12">
         <v>10</v>
       </c>
@@ -1557,8 +1573,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="12">
         <v>12</v>
       </c>
@@ -1567,8 +1583,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
-      <c r="B27" s="27"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="12">
         <v>13</v>
       </c>
@@ -1577,8 +1593,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
-      <c r="B28" s="27"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="12">
         <v>14</v>
       </c>
@@ -1587,8 +1603,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
-      <c r="B29" s="27"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="12">
         <v>15</v>
       </c>
@@ -1597,8 +1613,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="32"/>
-      <c r="B30" s="27" t="s">
+      <c r="A30" s="25"/>
+      <c r="B30" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="13">
@@ -1609,8 +1625,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="27"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="12">
         <v>4</v>
       </c>
@@ -1619,8 +1635,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="12">
         <v>5</v>
       </c>
@@ -1629,8 +1645,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="12">
         <v>6</v>
       </c>
@@ -1639,8 +1655,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="27"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="13">
         <v>7</v>
       </c>
@@ -1649,8 +1665,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
-      <c r="B35" s="27"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="12">
         <v>8</v>
       </c>
@@ -1659,8 +1675,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
-      <c r="B36" s="27"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="12">
         <v>10</v>
       </c>
@@ -1669,8 +1685,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="12">
         <v>11</v>
       </c>
@@ -1679,8 +1695,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="12">
         <v>12</v>
       </c>
@@ -1689,8 +1705,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
-      <c r="B39" s="27"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="12">
         <v>14</v>
       </c>
@@ -1699,7 +1715,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="11" t="s">
         <v>50</v>
       </c>
@@ -1711,8 +1727,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
-      <c r="B41" s="27" t="s">
+      <c r="A41" s="25"/>
+      <c r="B41" s="26" t="s">
         <v>52</v>
       </c>
       <c r="C41" s="12">
@@ -1723,8 +1739,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
-      <c r="B42" s="27"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="12">
         <v>4</v>
       </c>
@@ -1733,8 +1749,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="32"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="12">
         <v>5</v>
       </c>
@@ -1743,8 +1759,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="32"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="12">
         <v>8</v>
       </c>
@@ -1753,8 +1769,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="32"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="12">
         <v>9</v>
       </c>
@@ -1763,8 +1779,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="32"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="12">
         <v>10</v>
       </c>
@@ -1773,8 +1789,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="32"/>
-      <c r="B47" s="28" t="s">
+      <c r="A47" s="25"/>
+      <c r="B47" s="23" t="s">
         <v>60</v>
       </c>
       <c r="C47" s="15">
@@ -1785,8 +1801,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="32"/>
-      <c r="B48" s="28" t="s">
+      <c r="A48" s="25"/>
+      <c r="B48" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C48" s="15">
@@ -1797,8 +1813,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
-      <c r="B49" s="28" t="s">
+      <c r="A49" s="25"/>
+      <c r="B49" s="23" t="s">
         <v>62</v>
       </c>
       <c r="C49" s="15">
@@ -1809,8 +1825,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
-      <c r="B50" s="28" t="s">
+      <c r="A50" s="25"/>
+      <c r="B50" s="23" t="s">
         <v>63</v>
       </c>
       <c r="C50" s="15">
@@ -1821,7 +1837,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="32"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="16" t="s">
         <v>21</v>
       </c>
@@ -1833,8 +1849,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
-      <c r="B52" s="29" t="s">
+      <c r="A52" s="25"/>
+      <c r="B52" s="31" t="s">
         <v>65</v>
       </c>
       <c r="C52" s="20">
@@ -1845,8 +1861,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="32"/>
-      <c r="B53" s="29"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="31"/>
       <c r="C53" s="20">
         <v>5</v>
       </c>
@@ -1855,8 +1871,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="32"/>
-      <c r="B54" s="29"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="31"/>
       <c r="C54" s="19">
         <v>6</v>
       </c>
@@ -1865,8 +1881,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="32"/>
-      <c r="B55" s="29"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="31"/>
       <c r="C55" s="19">
         <v>7</v>
       </c>
@@ -1875,8 +1891,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="32"/>
-      <c r="B56" s="29"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="19">
         <v>8</v>
       </c>
@@ -1885,8 +1901,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
-      <c r="B57" s="29"/>
+      <c r="A57" s="25"/>
+      <c r="B57" s="31"/>
       <c r="C57" s="19">
         <v>9</v>
       </c>
@@ -1895,8 +1911,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="32"/>
-      <c r="B58" s="29"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="31"/>
       <c r="C58" s="19">
         <v>10</v>
       </c>
@@ -1905,8 +1921,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="32"/>
-      <c r="B59" s="29"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="19">
         <v>12</v>
       </c>
@@ -1915,8 +1931,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
-      <c r="B60" s="29"/>
+      <c r="A60" s="25"/>
+      <c r="B60" s="31"/>
       <c r="C60" s="19">
         <v>14</v>
       </c>
@@ -1925,8 +1941,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="32"/>
-      <c r="B61" s="29"/>
+      <c r="A61" s="25"/>
+      <c r="B61" s="31"/>
       <c r="C61" s="19">
         <v>15</v>
       </c>
@@ -1935,10 +1951,10 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="32" t="s">
+      <c r="A62" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B62" s="27" t="s">
+      <c r="B62" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C62" s="13">
@@ -1949,8 +1965,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="32"/>
-      <c r="B63" s="27"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="26"/>
       <c r="C63" s="13">
         <v>4</v>
       </c>
@@ -1959,8 +1975,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="32"/>
-      <c r="B64" s="27"/>
+      <c r="A64" s="25"/>
+      <c r="B64" s="26"/>
       <c r="C64" s="12">
         <v>5</v>
       </c>
@@ -1969,8 +1985,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
-      <c r="B65" s="27"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="12">
         <v>8</v>
       </c>
@@ -1979,8 +1995,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="32"/>
-      <c r="B66" s="27"/>
+      <c r="A66" s="25"/>
+      <c r="B66" s="26"/>
       <c r="C66" s="12">
         <v>10</v>
       </c>
@@ -1989,8 +2005,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="32"/>
-      <c r="B67" s="27"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="12">
         <v>12</v>
       </c>
@@ -1999,8 +2015,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="32"/>
-      <c r="B68" s="27"/>
+      <c r="A68" s="25"/>
+      <c r="B68" s="26"/>
       <c r="C68" s="12">
         <v>13</v>
       </c>
@@ -2009,8 +2025,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="32"/>
-      <c r="B69" s="27"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="12">
         <v>14</v>
       </c>
@@ -2019,8 +2035,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="32"/>
-      <c r="B70" s="27"/>
+      <c r="A70" s="25"/>
+      <c r="B70" s="26"/>
       <c r="C70" s="12">
         <v>15</v>
       </c>
@@ -2029,8 +2045,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="32"/>
-      <c r="B71" s="27" t="s">
+      <c r="A71" s="25"/>
+      <c r="B71" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C71" s="13">
@@ -2041,8 +2057,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="32"/>
-      <c r="B72" s="27"/>
+      <c r="A72" s="25"/>
+      <c r="B72" s="26"/>
       <c r="C72" s="12">
         <v>4</v>
       </c>
@@ -2051,8 +2067,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="32"/>
-      <c r="B73" s="27"/>
+      <c r="A73" s="25"/>
+      <c r="B73" s="26"/>
       <c r="C73" s="12">
         <v>5</v>
       </c>
@@ -2061,8 +2077,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="32"/>
-      <c r="B74" s="27"/>
+      <c r="A74" s="25"/>
+      <c r="B74" s="26"/>
       <c r="C74" s="12">
         <v>6</v>
       </c>
@@ -2071,8 +2087,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="32"/>
-      <c r="B75" s="27"/>
+      <c r="A75" s="25"/>
+      <c r="B75" s="26"/>
       <c r="C75" s="13">
         <v>7</v>
       </c>
@@ -2081,8 +2097,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="32"/>
-      <c r="B76" s="27"/>
+      <c r="A76" s="25"/>
+      <c r="B76" s="26"/>
       <c r="C76" s="12">
         <v>8</v>
       </c>
@@ -2091,8 +2107,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="32"/>
-      <c r="B77" s="27"/>
+      <c r="A77" s="25"/>
+      <c r="B77" s="26"/>
       <c r="C77" s="12">
         <v>10</v>
       </c>
@@ -2101,8 +2117,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="32"/>
-      <c r="B78" s="27"/>
+      <c r="A78" s="25"/>
+      <c r="B78" s="26"/>
       <c r="C78" s="12">
         <v>11</v>
       </c>
@@ -2111,8 +2127,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="32"/>
-      <c r="B79" s="27"/>
+      <c r="A79" s="25"/>
+      <c r="B79" s="26"/>
       <c r="C79" s="12">
         <v>12</v>
       </c>
@@ -2121,8 +2137,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="32"/>
-      <c r="B80" s="27"/>
+      <c r="A80" s="25"/>
+      <c r="B80" s="26"/>
       <c r="C80" s="12">
         <v>14</v>
       </c>
@@ -2131,7 +2147,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="32"/>
+      <c r="A81" s="25"/>
       <c r="B81" s="11" t="s">
         <v>50</v>
       </c>
@@ -2143,8 +2159,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="32"/>
-      <c r="B82" s="27" t="s">
+      <c r="A82" s="25"/>
+      <c r="B82" s="26" t="s">
         <v>52</v>
       </c>
       <c r="C82" s="12">
@@ -2155,8 +2171,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="32"/>
-      <c r="B83" s="27"/>
+      <c r="A83" s="25"/>
+      <c r="B83" s="26"/>
       <c r="C83" s="12">
         <v>4</v>
       </c>
@@ -2165,8 +2181,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="32"/>
-      <c r="B84" s="27"/>
+      <c r="A84" s="25"/>
+      <c r="B84" s="26"/>
       <c r="C84" s="12">
         <v>5</v>
       </c>
@@ -2175,8 +2191,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="32"/>
-      <c r="B85" s="27"/>
+      <c r="A85" s="25"/>
+      <c r="B85" s="26"/>
       <c r="C85" s="12">
         <v>8</v>
       </c>
@@ -2185,8 +2201,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
-      <c r="B86" s="27"/>
+      <c r="A86" s="25"/>
+      <c r="B86" s="26"/>
       <c r="C86" s="12">
         <v>9</v>
       </c>
@@ -2195,8 +2211,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="32"/>
-      <c r="B87" s="27"/>
+      <c r="A87" s="25"/>
+      <c r="B87" s="26"/>
       <c r="C87" s="12">
         <v>10</v>
       </c>
@@ -2204,22 +2220,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="32"/>
-      <c r="B88" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C88" s="15">
-        <v>5</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>59</v>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="25"/>
+      <c r="B88" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C88" s="17">
+        <v>3</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="32"/>
-      <c r="B89" s="28" t="s">
-        <v>61</v>
+      <c r="A89" s="25"/>
+      <c r="B89" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="C89" s="15">
         <v>5</v>
@@ -2229,9 +2245,9 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="32"/>
-      <c r="B90" s="28" t="s">
-        <v>62</v>
+      <c r="A90" s="25"/>
+      <c r="B90" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="C90" s="15">
         <v>5</v>
@@ -2241,9 +2257,9 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A91" s="32"/>
-      <c r="B91" s="28" t="s">
-        <v>63</v>
+      <c r="A91" s="25"/>
+      <c r="B91" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="C91" s="15">
         <v>5</v>
@@ -2252,23 +2268,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="32"/>
-      <c r="B92" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C92" s="17">
-        <v>3</v>
-      </c>
-      <c r="D92" s="16" t="s">
-        <v>22</v>
+    <row r="92" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="25"/>
+      <c r="B92" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" s="15">
+        <v>5</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="32" t="s">
+      <c r="A93" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="B93" s="27" t="s">
+      <c r="B93" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C93" s="13">
@@ -2279,8 +2295,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="32"/>
-      <c r="B94" s="27"/>
+      <c r="A94" s="25"/>
+      <c r="B94" s="26"/>
       <c r="C94" s="13">
         <v>4</v>
       </c>
@@ -2289,8 +2305,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="32"/>
-      <c r="B95" s="27"/>
+      <c r="A95" s="25"/>
+      <c r="B95" s="26"/>
       <c r="C95" s="12">
         <v>5</v>
       </c>
@@ -2299,8 +2315,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="32"/>
-      <c r="B96" s="27"/>
+      <c r="A96" s="25"/>
+      <c r="B96" s="26"/>
       <c r="C96" s="12">
         <v>8</v>
       </c>
@@ -2309,8 +2325,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="32"/>
-      <c r="B97" s="27"/>
+      <c r="A97" s="25"/>
+      <c r="B97" s="26"/>
       <c r="C97" s="12">
         <v>10</v>
       </c>
@@ -2319,8 +2335,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="32"/>
-      <c r="B98" s="27"/>
+      <c r="A98" s="25"/>
+      <c r="B98" s="26"/>
       <c r="C98" s="12">
         <v>12</v>
       </c>
@@ -2329,8 +2345,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="32"/>
-      <c r="B99" s="27"/>
+      <c r="A99" s="25"/>
+      <c r="B99" s="26"/>
       <c r="C99" s="12">
         <v>13</v>
       </c>
@@ -2339,8 +2355,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="32"/>
-      <c r="B100" s="27"/>
+      <c r="A100" s="25"/>
+      <c r="B100" s="26"/>
       <c r="C100" s="12">
         <v>14</v>
       </c>
@@ -2349,8 +2365,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="32"/>
-      <c r="B101" s="27"/>
+      <c r="A101" s="25"/>
+      <c r="B101" s="26"/>
       <c r="C101" s="12">
         <v>15</v>
       </c>
@@ -2359,8 +2375,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="32"/>
-      <c r="B102" s="27" t="s">
+      <c r="A102" s="25"/>
+      <c r="B102" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C102" s="13">
@@ -2371,8 +2387,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="32"/>
-      <c r="B103" s="27"/>
+      <c r="A103" s="25"/>
+      <c r="B103" s="26"/>
       <c r="C103" s="12">
         <v>4</v>
       </c>
@@ -2381,8 +2397,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="32"/>
-      <c r="B104" s="27"/>
+      <c r="A104" s="25"/>
+      <c r="B104" s="26"/>
       <c r="C104" s="12">
         <v>5</v>
       </c>
@@ -2391,8 +2407,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="32"/>
-      <c r="B105" s="27"/>
+      <c r="A105" s="25"/>
+      <c r="B105" s="26"/>
       <c r="C105" s="12">
         <v>6</v>
       </c>
@@ -2401,8 +2417,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="32"/>
-      <c r="B106" s="27"/>
+      <c r="A106" s="25"/>
+      <c r="B106" s="26"/>
       <c r="C106" s="13">
         <v>7</v>
       </c>
@@ -2411,8 +2427,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="32"/>
-      <c r="B107" s="27"/>
+      <c r="A107" s="25"/>
+      <c r="B107" s="26"/>
       <c r="C107" s="12">
         <v>8</v>
       </c>
@@ -2421,8 +2437,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="32"/>
-      <c r="B108" s="27"/>
+      <c r="A108" s="25"/>
+      <c r="B108" s="26"/>
       <c r="C108" s="12">
         <v>10</v>
       </c>
@@ -2431,8 +2447,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="32"/>
-      <c r="B109" s="27"/>
+      <c r="A109" s="25"/>
+      <c r="B109" s="26"/>
       <c r="C109" s="12">
         <v>11</v>
       </c>
@@ -2441,8 +2457,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="32"/>
-      <c r="B110" s="27"/>
+      <c r="A110" s="25"/>
+      <c r="B110" s="26"/>
       <c r="C110" s="12">
         <v>12</v>
       </c>
@@ -2451,8 +2467,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="32"/>
-      <c r="B111" s="27"/>
+      <c r="A111" s="25"/>
+      <c r="B111" s="26"/>
       <c r="C111" s="12">
         <v>14</v>
       </c>
@@ -2461,7 +2477,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="32"/>
+      <c r="A112" s="25"/>
       <c r="B112" s="11" t="s">
         <v>50</v>
       </c>
@@ -2473,8 +2489,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="32"/>
-      <c r="B113" s="27" t="s">
+      <c r="A113" s="25"/>
+      <c r="B113" s="26" t="s">
         <v>52</v>
       </c>
       <c r="C113" s="12">
@@ -2485,8 +2501,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="32"/>
-      <c r="B114" s="27"/>
+      <c r="A114" s="25"/>
+      <c r="B114" s="26"/>
       <c r="C114" s="12">
         <v>4</v>
       </c>
@@ -2495,8 +2511,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="32"/>
-      <c r="B115" s="27"/>
+      <c r="A115" s="25"/>
+      <c r="B115" s="26"/>
       <c r="C115" s="12">
         <v>5</v>
       </c>
@@ -2505,8 +2521,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="32"/>
-      <c r="B116" s="27"/>
+      <c r="A116" s="25"/>
+      <c r="B116" s="26"/>
       <c r="C116" s="12">
         <v>8</v>
       </c>
@@ -2515,8 +2531,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="32"/>
-      <c r="B117" s="27"/>
+      <c r="A117" s="25"/>
+      <c r="B117" s="26"/>
       <c r="C117" s="12">
         <v>9</v>
       </c>
@@ -2525,8 +2541,8 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="32"/>
-      <c r="B118" s="27"/>
+      <c r="A118" s="25"/>
+      <c r="B118" s="26"/>
       <c r="C118" s="12">
         <v>10</v>
       </c>
@@ -2534,10 +2550,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="32"/>
-      <c r="B119" s="28" t="s">
-        <v>60</v>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="25"/>
+      <c r="B119" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="C119" s="15">
         <v>5</v>
@@ -2546,10 +2562,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="32"/>
-      <c r="B120" s="28" t="s">
-        <v>61</v>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="25"/>
+      <c r="B120" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="C120" s="15">
         <v>5</v>
@@ -2558,10 +2574,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A121" s="32"/>
-      <c r="B121" s="28" t="s">
-        <v>62</v>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="25"/>
+      <c r="B121" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="C121" s="15">
         <v>5</v>
@@ -2570,10 +2586,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A122" s="32"/>
-      <c r="B122" s="28" t="s">
-        <v>63</v>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="25"/>
+      <c r="B122" s="23" t="s">
+        <v>88</v>
       </c>
       <c r="C122" s="15">
         <v>5</v>
@@ -2583,7 +2599,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="32"/>
+      <c r="A123" s="25"/>
       <c r="B123" s="16" t="s">
         <v>21</v>
       </c>
@@ -2595,7 +2611,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="30" t="s">
+      <c r="B124" s="32" t="s">
         <v>76</v>
       </c>
       <c r="C124" s="22">
@@ -2606,7 +2622,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="30"/>
+      <c r="B125" s="32"/>
       <c r="C125" s="22">
         <v>6</v>
       </c>
@@ -2615,7 +2631,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="30"/>
+      <c r="B126" s="32"/>
       <c r="C126" s="22">
         <v>7</v>
       </c>
@@ -2624,7 +2640,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="30" t="s">
+      <c r="B127" s="32" t="s">
         <v>80</v>
       </c>
       <c r="C127" s="22">
@@ -2635,7 +2651,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="30"/>
+      <c r="B128" s="32"/>
       <c r="C128" s="22">
         <v>6</v>
       </c>
@@ -2644,7 +2660,7 @@
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="30"/>
+      <c r="B129" s="32"/>
       <c r="C129" s="22">
         <v>7</v>
       </c>
@@ -2653,7 +2669,7 @@
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="31" t="s">
+      <c r="B130" s="33" t="s">
         <v>81</v>
       </c>
       <c r="C130" s="22">
@@ -2664,7 +2680,7 @@
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="31"/>
+      <c r="B131" s="33"/>
       <c r="C131" s="22">
         <v>6</v>
       </c>
@@ -2673,7 +2689,7 @@
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="31"/>
+      <c r="B132" s="33"/>
       <c r="C132" s="22">
         <v>7</v>
       </c>
@@ -2682,7 +2698,7 @@
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="30" t="s">
+      <c r="B133" s="32" t="s">
         <v>82</v>
       </c>
       <c r="C133" s="22">
@@ -2693,7 +2709,7 @@
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="30"/>
+      <c r="B134" s="32"/>
       <c r="C134" s="22">
         <v>6</v>
       </c>
@@ -2702,7 +2718,7 @@
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="30"/>
+      <c r="B135" s="32"/>
       <c r="C135" s="22">
         <v>7</v>
       </c>
@@ -2712,6 +2728,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="B124:B126"/>
+    <mergeCell ref="B133:B135"/>
+    <mergeCell ref="B130:B132"/>
+    <mergeCell ref="B127:B129"/>
+    <mergeCell ref="B71:B80"/>
+    <mergeCell ref="B82:B87"/>
     <mergeCell ref="A93:A123"/>
     <mergeCell ref="B93:B101"/>
     <mergeCell ref="B102:B111"/>
@@ -2728,13 +2751,6 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B21:B29"/>
     <mergeCell ref="B30:B39"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="B124:B126"/>
-    <mergeCell ref="B133:B135"/>
-    <mergeCell ref="B130:B132"/>
-    <mergeCell ref="B127:B129"/>
-    <mergeCell ref="B71:B80"/>
-    <mergeCell ref="B82:B87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>